<commit_message>
changed language of the game from czech to english and added some new words for the game
</commit_message>
<xml_diff>
--- a/test hangman/HangManV01/bin/Debug/Data - Excel/Words.xlsx
+++ b/test hangman/HangManV01/bin/Debug/Data - Excel/Words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kolko\Desktop\HANGMAN GAME DODELAT\test hangman\HangManV01\bin\Debug\Data - Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\Desktop\Git Hangman Hra\Hangman-Game\test hangman\HangManV01\bin\Debug\Data - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E004ECC0-D8F4-4F2F-BC03-31D086C17BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9068D34E-0650-43AE-A7F4-02BF283ABCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12960" yWindow="465" windowWidth="21120" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>aqw</t>
-  </si>
-  <si>
-    <t>qqq</t>
-  </si>
-  <si>
-    <t>fsadfdsa</t>
-  </si>
-  <si>
-    <t>fasfasd</t>
-  </si>
-  <si>
-    <t>yyy</t>
-  </si>
-  <si>
-    <t>gfd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>spider</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>kidney</t>
+  </si>
+  <si>
+    <t>Organ</t>
+  </si>
+  <si>
+    <t>moon</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>fountain</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>butterfly</t>
+  </si>
+  <si>
+    <t>insect</t>
+  </si>
+  <si>
+    <t>Umbrella</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>Necklace</t>
+  </si>
+  <si>
+    <t>Jewelry</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Guitar</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
@@ -360,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
@@ -392,6 +440,70 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>